<commit_message>
arreglado la busqueda pero la instalacion mas o menos
</commit_message>
<xml_diff>
--- a/electron-app/python/devices_report.xlsx
+++ b/electron-app/python/devices_report.xlsx
@@ -463,17 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>user</t>
+          <t>userdebug</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>N74E2L0132</t>
+          <t>ZY22KF33RF</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>15_V1UI35H.11-39-16</t>
+          <t>15_V1UIS35H.11-39-16-3</t>
         </is>
       </c>
     </row>

</xml_diff>